<commit_message>
screenshot ( in that case its have nothing happen when user can't login )
</commit_message>
<xml_diff>
--- a/AutomationSelenium/TestData/TestData.xlsx
+++ b/AutomationSelenium/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumTesting\AutomationSelenium\AutomationSelenium\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F2AF4A-47EF-477F-B381-CFD686450482}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15F3022-33FE-4D59-86AA-D2C0CE43D732}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{B242F0D5-C510-43E6-8665-29FA1A45120F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B242F0D5-C510-43E6-8665-29FA1A45120F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -420,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>123</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>